<commit_message>
Read data from openentrance platform
</commit_message>
<xml_diff>
--- a/project_open_entrance/01_external_data/scenarios/sets/aggregation/Years_interpolation.xlsx
+++ b/project_open_entrance/01_external_data/scenarios/sets/aggregation/Years_interpolation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boonmanhj\Documents\Gitlab\TNO-Eco-Mod-CI\project_open_entrance\01_external_data\scenarios\sets\aggregation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boonmanhj\Documents\Gitlab\tno-eco-mod-ci\project_open_entrance\01_external_data\scenarios\sets\aggregation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D34E0B-D9EC-4A90-939E-131D35FD03FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E8A992-BACF-4661-A0A8-8529BA57ABBD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Years_interpolation1" sheetId="5" r:id="rId1"/>
@@ -21,9 +21,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -576,7 +574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4906F231-CD2B-436D-9BC7-9C357742E490}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -978,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7337CF6-33DB-4BA9-9AE9-F2F8B2DF101F}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,7 +1395,7 @@
         <v>53</v>
       </c>
       <c r="K46">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>